<commit_message>
added users API details
</commit_message>
<xml_diff>
--- a/Library_Management.xlsx
+++ b/Library_Management.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\API\Library_Management_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358D8BFA-95A7-46AC-B2B6-560A5BE9B11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11E9809-E8B0-4188-8D09-D10E2E79DC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{97E855FB-80AE-482E-BDCC-C6E659E2F2CD}"/>
   </bookViews>
@@ -493,7 +493,7 @@
   <dimension ref="B3:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>